<commit_message>
Updates to include bar charts
Update to include bar charts requested my American Rivers.
</commit_message>
<xml_diff>
--- a/Data/De_river_states.xlsx
+++ b/Data/De_river_states.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\GitHub\DE_Basin_CWSRF_Analysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE0264C-9365-4176-9DF3-C84DC9FEE648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363B15FB-AA70-4D37-B51A-D545A74B6DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6633,10 +6633,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6648,6 +6650,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -6682,17 +6691,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6996,12 +7008,20 @@
   <dimension ref="A1:AX505"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="20.08984375" customWidth="1"/>
+    <col min="4" max="4" width="41.6328125" customWidth="1"/>
+    <col min="9" max="9" width="17.08984375" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="22.54296875" customWidth="1"/>
+    <col min="12" max="12" width="23.6328125" customWidth="1"/>
+    <col min="19" max="19" width="22.36328125" customWidth="1"/>
+    <col min="20" max="20" width="19.36328125" customWidth="1"/>
+    <col min="23" max="44" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.35">
@@ -62694,13 +62714,13 @@
       <c r="I379" s="2">
         <v>43571</v>
       </c>
-      <c r="J379">
+      <c r="J379" s="3">
         <v>3447464</v>
       </c>
       <c r="K379" s="2">
         <v>44923</v>
       </c>
-      <c r="L379">
+      <c r="L379" s="3">
         <v>2944366.51</v>
       </c>
       <c r="M379" t="s">
@@ -62843,7 +62863,7 @@
       <c r="I380" s="2">
         <v>43560</v>
       </c>
-      <c r="J380">
+      <c r="J380" s="3">
         <v>7188659</v>
       </c>
       <c r="K380" s="2">
@@ -62992,7 +63012,7 @@
       <c r="I381" s="2">
         <v>43560</v>
       </c>
-      <c r="J381">
+      <c r="J381" s="3">
         <v>163502</v>
       </c>
       <c r="K381" s="2">
@@ -63138,7 +63158,7 @@
       <c r="I382" s="2">
         <v>43560</v>
       </c>
-      <c r="J382">
+      <c r="J382" s="3">
         <v>285678</v>
       </c>
       <c r="K382" s="2">
@@ -63284,7 +63304,7 @@
       <c r="I383" s="2">
         <v>43559</v>
       </c>
-      <c r="J383">
+      <c r="J383" s="3">
         <v>7411107</v>
       </c>
       <c r="K383" s="2">
@@ -63433,7 +63453,7 @@
       <c r="I384" s="2">
         <v>43536</v>
       </c>
-      <c r="J384">
+      <c r="J384" s="3">
         <v>5686515</v>
       </c>
       <c r="K384" s="2">
@@ -63582,7 +63602,7 @@
       <c r="I385" s="2">
         <v>43524</v>
       </c>
-      <c r="J385">
+      <c r="J385" s="3">
         <v>1300000</v>
       </c>
       <c r="K385" s="2">
@@ -63731,7 +63751,7 @@
       <c r="I386" s="2">
         <v>43518</v>
       </c>
-      <c r="J386">
+      <c r="J386" s="3">
         <v>16634748</v>
       </c>
       <c r="K386" s="2">
@@ -63877,7 +63897,7 @@
       <c r="I387" s="2">
         <v>43517</v>
       </c>
-      <c r="J387">
+      <c r="J387" s="3">
         <v>10018681</v>
       </c>
       <c r="K387" s="2">
@@ -64023,7 +64043,7 @@
       <c r="I388" s="2">
         <v>43516</v>
       </c>
-      <c r="J388">
+      <c r="J388" s="3">
         <v>7176000</v>
       </c>
       <c r="K388" s="2">
@@ -64169,7 +64189,7 @@
       <c r="I389" s="2">
         <v>43515</v>
       </c>
-      <c r="J389">
+      <c r="J389" s="3">
         <v>9163512</v>
       </c>
       <c r="K389" s="2">
@@ -64315,7 +64335,7 @@
       <c r="I390" s="2">
         <v>43515</v>
       </c>
-      <c r="J390">
+      <c r="J390" s="3">
         <v>2263809</v>
       </c>
       <c r="K390" s="2">
@@ -64461,7 +64481,7 @@
       <c r="I391" s="2">
         <v>43509</v>
       </c>
-      <c r="J391">
+      <c r="J391" s="3">
         <v>100000</v>
       </c>
       <c r="K391" s="2">
@@ -64607,7 +64627,7 @@
       <c r="I392" s="2">
         <v>43509</v>
       </c>
-      <c r="J392">
+      <c r="J392" s="3">
         <v>1080036</v>
       </c>
       <c r="K392" s="2">
@@ -64753,7 +64773,7 @@
       <c r="I393" s="2">
         <v>43509</v>
       </c>
-      <c r="J393">
+      <c r="J393" s="3">
         <v>3861386</v>
       </c>
       <c r="K393" s="2">
@@ -64899,7 +64919,7 @@
       <c r="I394" s="2">
         <v>43509</v>
       </c>
-      <c r="J394">
+      <c r="J394" s="3">
         <v>6452222</v>
       </c>
       <c r="K394" s="2">
@@ -65045,7 +65065,7 @@
       <c r="I395" s="2">
         <v>43502</v>
       </c>
-      <c r="J395">
+      <c r="J395" s="3">
         <v>1625195</v>
       </c>
       <c r="K395" s="2">
@@ -65191,7 +65211,7 @@
       <c r="I396" s="2">
         <v>43502</v>
       </c>
-      <c r="J396">
+      <c r="J396" s="3">
         <v>332192</v>
       </c>
       <c r="K396" s="2">
@@ -65343,7 +65363,7 @@
       <c r="I397" s="2">
         <v>43496</v>
       </c>
-      <c r="J397">
+      <c r="J397" s="3">
         <v>6184000</v>
       </c>
       <c r="K397" s="2">
@@ -65492,7 +65512,7 @@
       <c r="I398" s="2">
         <v>43496</v>
       </c>
-      <c r="J398">
+      <c r="J398" s="3">
         <v>2458354</v>
       </c>
       <c r="K398" s="2">
@@ -65641,7 +65661,7 @@
       <c r="I399" s="2">
         <v>43474</v>
       </c>
-      <c r="J399">
+      <c r="J399" s="3">
         <v>301820</v>
       </c>
       <c r="K399" s="2">
@@ -65793,7 +65813,7 @@
       <c r="I400" s="2">
         <v>43468</v>
       </c>
-      <c r="J400">
+      <c r="J400" s="3">
         <v>11695000</v>
       </c>
       <c r="K400" s="2">
@@ -65942,7 +65962,7 @@
       <c r="I401" s="2">
         <v>43455</v>
       </c>
-      <c r="J401">
+      <c r="J401" s="3">
         <v>4132550</v>
       </c>
       <c r="K401" s="2">
@@ -66088,7 +66108,7 @@
       <c r="I402" s="2">
         <v>43455</v>
       </c>
-      <c r="J402">
+      <c r="J402" s="3">
         <v>1985572</v>
       </c>
       <c r="K402" s="2">
@@ -66237,7 +66257,7 @@
       <c r="I403" s="2">
         <v>43454</v>
       </c>
-      <c r="J403">
+      <c r="J403" s="3">
         <v>5049505</v>
       </c>
       <c r="K403" s="2">
@@ -66386,7 +66406,7 @@
       <c r="I404" s="2">
         <v>43453</v>
       </c>
-      <c r="J404">
+      <c r="J404" s="3">
         <v>1705275</v>
       </c>
       <c r="K404" s="2">
@@ -66532,7 +66552,7 @@
       <c r="I405" s="2">
         <v>43452</v>
       </c>
-      <c r="J405">
+      <c r="J405" s="3">
         <v>1729561</v>
       </c>
       <c r="K405" s="2">
@@ -66678,7 +66698,7 @@
       <c r="I406" s="2">
         <v>43452</v>
       </c>
-      <c r="J406">
+      <c r="J406" s="3">
         <v>159456</v>
       </c>
       <c r="K406" s="2">
@@ -66827,7 +66847,7 @@
       <c r="I407" s="2">
         <v>43452</v>
       </c>
-      <c r="J407">
+      <c r="J407" s="3">
         <v>10900000</v>
       </c>
       <c r="K407" s="2">
@@ -66973,7 +66993,7 @@
       <c r="I408" s="2">
         <v>43452</v>
       </c>
-      <c r="J408">
+      <c r="J408" s="3">
         <v>1560675</v>
       </c>
       <c r="K408" s="2">
@@ -67119,13 +67139,13 @@
       <c r="I409" s="2">
         <v>43446</v>
       </c>
-      <c r="J409">
+      <c r="J409" s="3">
         <v>4888205</v>
       </c>
       <c r="K409" s="2">
         <v>44923</v>
       </c>
-      <c r="L409">
+      <c r="L409" s="3">
         <v>4313473.2300000004</v>
       </c>
       <c r="M409" t="s">
@@ -67268,7 +67288,7 @@
       <c r="I410" s="2">
         <v>43440</v>
       </c>
-      <c r="J410">
+      <c r="J410" s="3">
         <v>307000</v>
       </c>
       <c r="K410" s="2">
@@ -67420,7 +67440,7 @@
       <c r="I411" s="2">
         <v>43433</v>
       </c>
-      <c r="J411">
+      <c r="J411" s="3">
         <v>1058100</v>
       </c>
       <c r="K411" s="2">
@@ -67569,7 +67589,7 @@
       <c r="I412" s="2">
         <v>43431</v>
       </c>
-      <c r="J412">
+      <c r="J412" s="3">
         <v>9000000</v>
       </c>
       <c r="K412" s="2">
@@ -67718,7 +67738,7 @@
       <c r="I413" s="2">
         <v>43424</v>
       </c>
-      <c r="J413">
+      <c r="J413" s="3">
         <v>11136900</v>
       </c>
       <c r="K413" s="2">
@@ -67867,7 +67887,7 @@
       <c r="I414" s="2">
         <v>43411</v>
       </c>
-      <c r="J414">
+      <c r="J414" s="3">
         <v>2538000</v>
       </c>
       <c r="K414" s="2">
@@ -68010,7 +68030,7 @@
       <c r="I415" s="2">
         <v>43410</v>
       </c>
-      <c r="J415">
+      <c r="J415" s="3">
         <v>904994</v>
       </c>
       <c r="K415" s="2">
@@ -68159,7 +68179,7 @@
       <c r="I416" s="2">
         <v>43405</v>
       </c>
-      <c r="J416">
+      <c r="J416" s="3">
         <v>2315000</v>
       </c>
       <c r="K416" s="2">
@@ -68305,7 +68325,7 @@
       <c r="I417" s="2">
         <v>43404</v>
       </c>
-      <c r="J417">
+      <c r="J417" s="3">
         <v>1370760</v>
       </c>
       <c r="K417" s="2">
@@ -68454,7 +68474,7 @@
       <c r="I418" s="2">
         <v>43403</v>
       </c>
-      <c r="J418">
+      <c r="J418" s="3">
         <v>1200000</v>
       </c>
       <c r="K418" s="2">
@@ -68603,7 +68623,7 @@
       <c r="I419" s="2">
         <v>43398</v>
       </c>
-      <c r="J419">
+      <c r="J419" s="3">
         <v>11957204</v>
       </c>
       <c r="K419" s="2">
@@ -68746,7 +68766,7 @@
       <c r="I420" s="2">
         <v>43398</v>
       </c>
-      <c r="J420">
+      <c r="J420" s="3">
         <v>17326733</v>
       </c>
       <c r="K420" s="2">
@@ -68892,7 +68912,7 @@
       <c r="I421" s="2">
         <v>43396</v>
       </c>
-      <c r="J421">
+      <c r="J421" s="3">
         <v>2187935</v>
       </c>
       <c r="K421" s="2">
@@ -69038,13 +69058,13 @@
       <c r="I422" s="2">
         <v>43391</v>
       </c>
-      <c r="J422">
+      <c r="J422" s="3">
         <v>4822315</v>
       </c>
       <c r="K422" s="2">
         <v>44923</v>
       </c>
-      <c r="L422">
+      <c r="L422" s="3">
         <v>3888289.04</v>
       </c>
       <c r="M422" t="s">
@@ -69187,7 +69207,7 @@
       <c r="I423" s="2">
         <v>43382</v>
       </c>
-      <c r="J423">
+      <c r="J423" s="3">
         <v>618150</v>
       </c>
       <c r="K423" s="2">

</xml_diff>